<commit_message>
add optimized csv and potential impact assessment
</commit_message>
<xml_diff>
--- a/data/phone_transcripts_v0.1.xlsx
+++ b/data/phone_transcripts_v0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alpay\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev_projects_pc\transcript-dashboard-ai\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB75A89F-4A1A-4DE5-97EA-B1706CB1EC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA26246-18F2-47AF-9C16-A19D9C9A9191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10605" yWindow="4860" windowWidth="38700" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="159">
   <si>
     <t>CallID</t>
   </si>
@@ -32,303 +32,6 @@
   </si>
   <si>
     <t>Transcript</t>
-  </si>
-  <si>
-    <t>15/01/2025</t>
-  </si>
-  <si>
-    <t>20/02/2025</t>
-  </si>
-  <si>
-    <t>10/03/2025</t>
-  </si>
-  <si>
-    <t>05/04/2025</t>
-  </si>
-  <si>
-    <t>22/05/2025</t>
-  </si>
-  <si>
-    <t>18/06/2025</t>
-  </si>
-  <si>
-    <t>09/07/2025</t>
-  </si>
-  <si>
-    <t>14/08/2025</t>
-  </si>
-  <si>
-    <t>25/09/2025</t>
-  </si>
-  <si>
-    <t>30/10/2025</t>
-  </si>
-  <si>
-    <t>03/11/2024</t>
-  </si>
-  <si>
-    <t>18/12/2024</t>
-  </si>
-  <si>
-    <t>07/01/2024</t>
-  </si>
-  <si>
-    <t>21/02/2024</t>
-  </si>
-  <si>
-    <t>14/03/2024</t>
-  </si>
-  <si>
-    <t>29/04/2024</t>
-  </si>
-  <si>
-    <t>11/05/2024</t>
-  </si>
-  <si>
-    <t>26/06/2024</t>
-  </si>
-  <si>
-    <t>09/07/2024</t>
-  </si>
-  <si>
-    <t>24/08/2024</t>
-  </si>
-  <si>
-    <t>16/09/2024</t>
-  </si>
-  <si>
-    <t>31/10/2024</t>
-  </si>
-  <si>
-    <t>13/11/2024</t>
-  </si>
-  <si>
-    <t>28/12/2024</t>
-  </si>
-  <si>
-    <t>10/01/2023</t>
-  </si>
-  <si>
-    <t>25/02/2023</t>
-  </si>
-  <si>
-    <t>19/03/2023</t>
-  </si>
-  <si>
-    <t>04/04/2023</t>
-  </si>
-  <si>
-    <t>29/05/2023</t>
-  </si>
-  <si>
-    <t>11/06/2023</t>
-  </si>
-  <si>
-    <t>26/07/2023</t>
-  </si>
-  <si>
-    <t>08/08/2023</t>
-  </si>
-  <si>
-    <t>23/09/2023</t>
-  </si>
-  <si>
-    <t>15/10/2023</t>
-  </si>
-  <si>
-    <t>30/11/2023</t>
-  </si>
-  <si>
-    <t>12/12/2023</t>
-  </si>
-  <si>
-    <t>27/01/2025</t>
-  </si>
-  <si>
-    <t>09/02/2025</t>
-  </si>
-  <si>
-    <t>24/03/2025</t>
-  </si>
-  <si>
-    <t>06/04/2025</t>
-  </si>
-  <si>
-    <t>21/05/2025</t>
-  </si>
-  <si>
-    <t>03/06/2025</t>
-  </si>
-  <si>
-    <t>18/07/2025</t>
-  </si>
-  <si>
-    <t>30/08/2025</t>
-  </si>
-  <si>
-    <t>12/09/2025</t>
-  </si>
-  <si>
-    <t>27/10/2025</t>
-  </si>
-  <si>
-    <t>09/11/2024</t>
-  </si>
-  <si>
-    <t>24/12/2024</t>
-  </si>
-  <si>
-    <t>16/01/2024</t>
-  </si>
-  <si>
-    <t>01/02/2024</t>
-  </si>
-  <si>
-    <t>18/03/2024</t>
-  </si>
-  <si>
-    <t>02/04/2024</t>
-  </si>
-  <si>
-    <t>17/05/2024</t>
-  </si>
-  <si>
-    <t>29/06/2024</t>
-  </si>
-  <si>
-    <t>11/07/2024</t>
-  </si>
-  <si>
-    <t>26/08/2024</t>
-  </si>
-  <si>
-    <t>08/09/2024</t>
-  </si>
-  <si>
-    <t>23/10/2024</t>
-  </si>
-  <si>
-    <t>05/11/2024</t>
-  </si>
-  <si>
-    <t>20/12/2024</t>
-  </si>
-  <si>
-    <t>02/01/2023</t>
-  </si>
-  <si>
-    <t>17/02/2023</t>
-  </si>
-  <si>
-    <t>01/03/2023</t>
-  </si>
-  <si>
-    <t>16/04/2023</t>
-  </si>
-  <si>
-    <t>28/05/2023</t>
-  </si>
-  <si>
-    <t>10/06/2023</t>
-  </si>
-  <si>
-    <t>25/07/2023</t>
-  </si>
-  <si>
-    <t>07/08/2023</t>
-  </si>
-  <si>
-    <t>22/09/2023</t>
-  </si>
-  <si>
-    <t>04/10/2023</t>
-  </si>
-  <si>
-    <t>19/11/2023</t>
-  </si>
-  <si>
-    <t>01/12/2023</t>
-  </si>
-  <si>
-    <t>14/01/2025</t>
-  </si>
-  <si>
-    <t>26/02/2025</t>
-  </si>
-  <si>
-    <t>25/04/2025</t>
-  </si>
-  <si>
-    <t>07/05/2025</t>
-  </si>
-  <si>
-    <t>22/06/2025</t>
-  </si>
-  <si>
-    <t>04/07/2025</t>
-  </si>
-  <si>
-    <t>19/08/2025</t>
-  </si>
-  <si>
-    <t>01/09/2025</t>
-  </si>
-  <si>
-    <t>16/10/2025</t>
-  </si>
-  <si>
-    <t>28/11/2024</t>
-  </si>
-  <si>
-    <t>10/12/2024</t>
-  </si>
-  <si>
-    <t>25/01/2024</t>
-  </si>
-  <si>
-    <t>07/02/2024</t>
-  </si>
-  <si>
-    <t>22/03/2024</t>
-  </si>
-  <si>
-    <t>04/04/2024</t>
-  </si>
-  <si>
-    <t>19/05/2024</t>
-  </si>
-  <si>
-    <t>01/06/2024</t>
-  </si>
-  <si>
-    <t>16/07/2024</t>
-  </si>
-  <si>
-    <t>28/08/2024</t>
-  </si>
-  <si>
-    <t>10/09/2024</t>
-  </si>
-  <si>
-    <t>25/10/2024</t>
-  </si>
-  <si>
-    <t>07/11/2024</t>
-  </si>
-  <si>
-    <t>22/12/2024</t>
-  </si>
-  <si>
-    <t>04/01/2023</t>
-  </si>
-  <si>
-    <t>19/02/2023</t>
-  </si>
-  <si>
-    <t>03/03/2023</t>
-  </si>
-  <si>
-    <t>18/04/2023</t>
   </si>
   <si>
     <t>06:32:00</t>
@@ -800,6 +503,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -852,11 +558,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1161,19 +871,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1182,1407 +895,1405 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3">
+        <v>45672</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
       <c r="D2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3">
+        <v>45708</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>104</v>
-      </c>
       <c r="D3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3">
+        <v>45726</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>105</v>
-      </c>
       <c r="D4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3">
+        <v>45752</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
       <c r="D5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3">
+        <v>45799</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
       <c r="D6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3">
+        <v>45826</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>108</v>
-      </c>
       <c r="D7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3">
+        <v>45847</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>109</v>
-      </c>
       <c r="D8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>110</v>
-      </c>
       <c r="D9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
       <c r="D10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3">
+        <v>45960</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>112</v>
-      </c>
       <c r="D11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3">
+        <v>45599</v>
+      </c>
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
       <c r="D12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3">
+        <v>45644</v>
+      </c>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>114</v>
-      </c>
       <c r="D13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3">
+        <v>45298</v>
+      </c>
+      <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>115</v>
-      </c>
       <c r="D14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3">
+        <v>45343</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>116</v>
-      </c>
       <c r="D15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3">
+        <v>45365</v>
+      </c>
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
       <c r="D16" t="s">
-        <v>172</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3">
+        <v>45411</v>
+      </c>
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
       <c r="D17" t="s">
-        <v>173</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3">
+        <v>45423</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
-        <v>119</v>
-      </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3">
+        <v>45469</v>
+      </c>
+      <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
-        <v>120</v>
-      </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3">
+        <v>45482</v>
+      </c>
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
-        <v>121</v>
-      </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3">
+        <v>45528</v>
+      </c>
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
-        <v>122</v>
-      </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3">
+        <v>45551</v>
+      </c>
+      <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
-        <v>123</v>
-      </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3">
+        <v>45596</v>
+      </c>
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
-        <v>124</v>
-      </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3">
+        <v>45609</v>
+      </c>
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
-        <v>125</v>
-      </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3">
+        <v>45654</v>
+      </c>
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="C25" t="s">
-        <v>126</v>
-      </c>
       <c r="D25" t="s">
-        <v>181</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3">
+        <v>44936</v>
+      </c>
+      <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" t="s">
-        <v>127</v>
-      </c>
       <c r="D26" t="s">
-        <v>182</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3">
+        <v>44982</v>
+      </c>
+      <c r="C27" t="s">
         <v>29</v>
       </c>
-      <c r="C27" t="s">
-        <v>128</v>
-      </c>
       <c r="D27" t="s">
-        <v>183</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3">
+        <v>45004</v>
+      </c>
+      <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
-        <v>129</v>
-      </c>
       <c r="D28" t="s">
-        <v>184</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3">
+        <v>45020</v>
+      </c>
+      <c r="C29" t="s">
         <v>31</v>
       </c>
-      <c r="C29" t="s">
-        <v>130</v>
-      </c>
       <c r="D29" t="s">
-        <v>185</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3">
+        <v>45075</v>
+      </c>
+      <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="C30" t="s">
-        <v>131</v>
-      </c>
       <c r="D30" t="s">
-        <v>186</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3">
+        <v>45088</v>
+      </c>
+      <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="C31" t="s">
-        <v>132</v>
-      </c>
       <c r="D31" t="s">
-        <v>187</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3">
+        <v>45133</v>
+      </c>
+      <c r="C32" t="s">
         <v>34</v>
       </c>
-      <c r="C32" t="s">
-        <v>133</v>
-      </c>
       <c r="D32" t="s">
-        <v>188</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3">
+        <v>45146</v>
+      </c>
+      <c r="C33" t="s">
         <v>35</v>
       </c>
-      <c r="C33" t="s">
-        <v>134</v>
-      </c>
       <c r="D33" t="s">
-        <v>189</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3">
+        <v>45192</v>
+      </c>
+      <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="C34" t="s">
-        <v>135</v>
-      </c>
       <c r="D34" t="s">
-        <v>190</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3">
+        <v>45214</v>
+      </c>
+      <c r="C35" t="s">
         <v>37</v>
       </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
       <c r="D35" t="s">
-        <v>191</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3">
+        <v>45260</v>
+      </c>
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="C36" t="s">
-        <v>137</v>
-      </c>
       <c r="D36" t="s">
-        <v>192</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>39</v>
+      <c r="B37" s="3">
+        <v>45272</v>
       </c>
       <c r="C37" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>193</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>40</v>
+      <c r="B38" s="3">
+        <v>45684</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="D38" t="s">
-        <v>194</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
-        <v>41</v>
+      <c r="B39" s="3">
+        <v>45697</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>195</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
-        <v>42</v>
+      <c r="B40" s="3">
+        <v>45740</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
-        <v>43</v>
+      <c r="B41" s="3">
+        <v>45753</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
-        <v>44</v>
+      <c r="B42" s="3">
+        <v>45798</v>
       </c>
       <c r="C42" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>198</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
-        <v>45</v>
+      <c r="B43" s="3">
+        <v>45811</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>199</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
-        <v>46</v>
+      <c r="B44" s="3">
+        <v>45856</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="D44" t="s">
-        <v>200</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
-        <v>47</v>
+      <c r="B45" s="3">
+        <v>45899</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>201</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>48</v>
+      <c r="B46" s="3">
+        <v>45912</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>202</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
-        <v>49</v>
+      <c r="B47" s="3">
+        <v>45957</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>203</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
-        <v>50</v>
+      <c r="B48" s="3">
+        <v>45605</v>
       </c>
       <c r="C48" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>204</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
-        <v>51</v>
+      <c r="B49" s="3">
+        <v>45650</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>205</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
-        <v>52</v>
+      <c r="B50" s="3">
+        <v>45307</v>
       </c>
       <c r="C50" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="D50" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
-        <v>53</v>
+      <c r="B51" s="3">
+        <v>45323</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D51" t="s">
-        <v>207</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
-        <v>54</v>
+      <c r="B52" s="3">
+        <v>45369</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="D52" t="s">
-        <v>208</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
-        <v>55</v>
+      <c r="B53" s="3">
+        <v>45384</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>209</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
-        <v>56</v>
+      <c r="B54" s="3">
+        <v>45429</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>210</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
-        <v>57</v>
+      <c r="B55" s="3">
+        <v>45472</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>211</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
-        <v>58</v>
+      <c r="B56" s="3">
+        <v>45484</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>212</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>59</v>
+      <c r="B57" s="3">
+        <v>45530</v>
       </c>
       <c r="C57" t="s">
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="D57" t="s">
-        <v>213</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
-        <v>60</v>
+      <c r="B58" s="3">
+        <v>45543</v>
       </c>
       <c r="C58" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
       <c r="D58" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
-        <v>61</v>
+      <c r="B59" s="3">
+        <v>45588</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="D59" t="s">
-        <v>215</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
-        <v>62</v>
+      <c r="B60" s="3">
+        <v>45601</v>
       </c>
       <c r="C60" t="s">
-        <v>131</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s">
-        <v>216</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
-        <v>63</v>
+      <c r="B61" s="3">
+        <v>45646</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
       <c r="D61" t="s">
-        <v>217</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
-        <v>64</v>
+      <c r="B62" s="3">
+        <v>44928</v>
       </c>
       <c r="C62" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>218</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
-        <v>65</v>
+      <c r="B63" s="3">
+        <v>44974</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
       <c r="D63" t="s">
-        <v>219</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
-        <v>66</v>
+      <c r="B64" s="3">
+        <v>44986</v>
       </c>
       <c r="C64" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="D64" t="s">
-        <v>220</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>67</v>
+      <c r="B65" s="3">
+        <v>45032</v>
       </c>
       <c r="C65" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>221</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
-        <v>68</v>
+      <c r="B66" s="3">
+        <v>45074</v>
       </c>
       <c r="C66" t="s">
-        <v>150</v>
+        <v>51</v>
       </c>
       <c r="D66" t="s">
-        <v>222</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
-        <v>69</v>
+      <c r="B67" s="3">
+        <v>45087</v>
       </c>
       <c r="C67" t="s">
-        <v>120</v>
+        <v>21</v>
       </c>
       <c r="D67" t="s">
-        <v>223</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
-        <v>70</v>
+      <c r="B68" s="3">
+        <v>45132</v>
       </c>
       <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" t="s">
         <v>125</v>
-      </c>
-      <c r="D68" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
-        <v>71</v>
+      <c r="B69" s="3">
+        <v>45145</v>
       </c>
       <c r="C69" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" t="s">
         <v>126</v>
-      </c>
-      <c r="D69" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
-        <v>72</v>
+      <c r="B70" s="3">
+        <v>45191</v>
       </c>
       <c r="C70" t="s">
+        <v>28</v>
+      </c>
+      <c r="D70" t="s">
         <v>127</v>
-      </c>
-      <c r="D70" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
-        <v>73</v>
+      <c r="B71" s="3">
+        <v>45203</v>
       </c>
       <c r="C71" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="D71" t="s">
-        <v>227</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
-        <v>74</v>
+      <c r="B72" s="3">
+        <v>45249</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>39</v>
       </c>
       <c r="D72" t="s">
-        <v>228</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
-        <v>75</v>
+      <c r="B73" s="3">
+        <v>45261</v>
       </c>
       <c r="C73" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="D73" t="s">
-        <v>229</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
-        <v>76</v>
+      <c r="B74" s="3">
+        <v>45671</v>
       </c>
       <c r="C74" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="D74" t="s">
-        <v>230</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
-        <v>77</v>
+      <c r="B75" s="3">
+        <v>45714</v>
       </c>
       <c r="C75" t="s">
-        <v>151</v>
+        <v>52</v>
       </c>
       <c r="D75" t="s">
-        <v>231</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
-        <v>6</v>
+      <c r="B76" s="3">
+        <v>45726</v>
       </c>
       <c r="C76" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
       <c r="D76" t="s">
-        <v>232</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
-        <v>78</v>
+      <c r="B77" s="3">
+        <v>45772</v>
       </c>
       <c r="C77" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="D77" t="s">
-        <v>233</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
-        <v>79</v>
+      <c r="B78" s="3">
+        <v>45784</v>
       </c>
       <c r="C78" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="D78" t="s">
-        <v>234</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
-        <v>80</v>
+      <c r="B79" s="3">
+        <v>45830</v>
       </c>
       <c r="C79" t="s">
-        <v>152</v>
+        <v>53</v>
       </c>
       <c r="D79" t="s">
-        <v>235</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
-        <v>81</v>
+      <c r="B80" s="3">
+        <v>45842</v>
       </c>
       <c r="C80" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="D80" t="s">
-        <v>236</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
-        <v>82</v>
+      <c r="B81" s="3">
+        <v>45888</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>54</v>
       </c>
       <c r="D81" t="s">
-        <v>237</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
-        <v>83</v>
+      <c r="B82" s="3">
+        <v>45901</v>
       </c>
       <c r="C82" t="s">
-        <v>135</v>
+        <v>36</v>
       </c>
       <c r="D82" t="s">
-        <v>238</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
-        <v>84</v>
+      <c r="B83" s="3">
+        <v>45946</v>
       </c>
       <c r="C83" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D83" t="s">
-        <v>239</v>
+        <v>140</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
-        <v>85</v>
+      <c r="B84" s="3">
+        <v>45624</v>
       </c>
       <c r="C84" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>240</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" t="s">
-        <v>86</v>
+      <c r="B85" s="3">
+        <v>45636</v>
       </c>
       <c r="C85" t="s">
-        <v>154</v>
+        <v>55</v>
       </c>
       <c r="D85" t="s">
-        <v>241</v>
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
-        <v>87</v>
+      <c r="B86" s="3">
+        <v>45316</v>
       </c>
       <c r="C86" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="D86" t="s">
-        <v>242</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" t="s">
-        <v>88</v>
+      <c r="B87" s="3">
+        <v>45329</v>
       </c>
       <c r="C87" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D87" t="s">
-        <v>243</v>
+        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="B88" t="s">
-        <v>89</v>
+      <c r="B88" s="3">
+        <v>45373</v>
       </c>
       <c r="C88" t="s">
-        <v>133</v>
+        <v>34</v>
       </c>
       <c r="D88" t="s">
-        <v>244</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
-      <c r="B89" t="s">
-        <v>90</v>
+      <c r="B89" s="3">
+        <v>45386</v>
       </c>
       <c r="C89" t="s">
-        <v>130</v>
+        <v>31</v>
       </c>
       <c r="D89" t="s">
-        <v>245</v>
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
-      <c r="B90" t="s">
-        <v>91</v>
+      <c r="B90" s="3">
+        <v>45431</v>
       </c>
       <c r="C90" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="D90" t="s">
-        <v>246</v>
+        <v>147</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
-      <c r="B91" t="s">
-        <v>92</v>
+      <c r="B91" s="3">
+        <v>45444</v>
       </c>
       <c r="C91" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="D91" t="s">
-        <v>247</v>
+        <v>148</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
-        <v>93</v>
+      <c r="B92" s="3">
+        <v>45489</v>
       </c>
       <c r="C92" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="D92" t="s">
-        <v>248</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
-        <v>94</v>
+      <c r="B93" s="3">
+        <v>45532</v>
       </c>
       <c r="C93" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="D93" t="s">
-        <v>249</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
-      <c r="B94" t="s">
-        <v>95</v>
+      <c r="B94" s="3">
+        <v>45545</v>
       </c>
       <c r="C94" t="s">
-        <v>131</v>
+        <v>32</v>
       </c>
       <c r="D94" t="s">
-        <v>250</v>
+        <v>151</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
-      <c r="B95" t="s">
-        <v>96</v>
+      <c r="B95" s="3">
+        <v>45590</v>
       </c>
       <c r="C95" t="s">
-        <v>112</v>
+        <v>13</v>
       </c>
       <c r="D95" t="s">
-        <v>251</v>
+        <v>152</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
-      <c r="B96" t="s">
-        <v>97</v>
+      <c r="B96" s="3">
+        <v>45603</v>
       </c>
       <c r="C96" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="D96" t="s">
-        <v>252</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
-      <c r="B97" t="s">
-        <v>98</v>
+      <c r="B97" s="3">
+        <v>45648</v>
       </c>
       <c r="C97" t="s">
-        <v>134</v>
+        <v>35</v>
       </c>
       <c r="D97" t="s">
-        <v>253</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
-      <c r="B98" t="s">
-        <v>99</v>
+      <c r="B98" s="3">
+        <v>44930</v>
       </c>
       <c r="C98" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="D98" t="s">
-        <v>254</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
-        <v>100</v>
+      <c r="B99" s="3">
+        <v>44976</v>
       </c>
       <c r="C99" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="D99" t="s">
-        <v>255</v>
+        <v>156</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
-      <c r="B100" t="s">
-        <v>101</v>
+      <c r="B100" s="3">
+        <v>44988</v>
       </c>
       <c r="C100" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="D100" t="s">
-        <v>256</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
-      <c r="B101" t="s">
-        <v>102</v>
+      <c r="B101" s="3">
+        <v>45034</v>
       </c>
       <c r="C101" t="s">
-        <v>120</v>
+        <v>21</v>
       </c>
       <c r="D101" t="s">
-        <v>257</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>